<commit_message>
Modified part number for header in SMT dummy cell.
</commit_message>
<xml_diff>
--- a/hardware/pcbs/dummy_cell/smt/smt_50k/gerber/fab/BOM_JLCPCB.xlsx
+++ b/hardware/pcbs/dummy_cell/smt/smt_50k/gerber/fab/BOM_JLCPCB.xlsx
@@ -117,7 +117,7 @@
     <t xml:space="preserve">NA</t>
   </si>
   <si>
-    <t xml:space="preserve">C9900026232</t>
+    <t xml:space="preserve">C5197650</t>
   </si>
 </sst>
 </file>
@@ -359,7 +359,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>